<commit_message>
Blank size changes and Colors added
</commit_message>
<xml_diff>
--- a/Quick Ship Router/bin/Debug/Summary Sheet.xlsx
+++ b/Quick Ship Router/bin/Debug/Summary Sheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15525" windowHeight="11595"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15525" windowHeight="11595" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary Template" sheetId="1" r:id="rId1"/>
@@ -72,13 +72,13 @@
     <t>Labor</t>
   </si>
   <si>
-    <t>total (min)</t>
-  </si>
-  <si>
     <t>Blanks</t>
   </si>
   <si>
     <t>P=Produce; I=Inventory</t>
+  </si>
+  <si>
+    <t>total (hours)</t>
   </si>
 </sst>
 </file>
@@ -228,6 +228,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -238,9 +241,6 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -525,7 +525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -544,22 +544,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="20" t="s">
-        <v>17</v>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="16" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -600,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -610,18 +610,18 @@
     <col min="2" max="2" width="13.7109375" style="11" customWidth="1"/>
     <col min="3" max="3" width="8" style="5" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="D1" s="19" t="s">
+      <c r="A1" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="D1" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="19"/>
+      <c r="E1" s="20"/>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
     </row>
@@ -630,7 +630,7 @@
       <c r="B2" s="10"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="12" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
@@ -641,7 +641,7 @@
         <v>14</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Pallets added, and CSV referencing
</commit_message>
<xml_diff>
--- a/Quick Ship Router/bin/Debug/Summary Sheet.xlsx
+++ b/Quick Ship Router/bin/Debug/Summary Sheet.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Item Code</t>
   </si>
@@ -79,6 +79,15 @@
   </si>
   <si>
     <t>total (hours)</t>
+  </si>
+  <si>
+    <t>Pallets</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Approx Qty</t>
   </si>
 </sst>
 </file>
@@ -183,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -197,26 +206,8 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -231,6 +222,18 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -239,9 +242,6 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -544,21 +544,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="6"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="16" t="s">
+      <c r="A2" s="5"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="10" t="s">
         <v>16</v>
       </c>
     </row>
@@ -601,71 +601,85 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="11" customWidth="1"/>
-    <col min="3" max="3" width="8" style="5" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="21" style="9" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="1.5703125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="1.42578125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="D1" s="20" t="s">
+      <c r="B1" s="17"/>
+      <c r="D1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="E1" s="17"/>
+      <c r="G1" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="10"/>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" spans="1:8" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="C3" s="13"/>
       <c r="D3" s="8" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>17</v>
       </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="14"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="9"/>
+      <c r="E5" s="14"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="9"/>
+      <c r="E6" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>